<commit_message>
Adding parameters for stylesheet
</commit_message>
<xml_diff>
--- a/metadata/cdisc_collection_forms.xlsx
+++ b/metadata/cdisc_collection_forms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\lexjansen\cdisc360i-pocs\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D91CAB-6E56-474E-B969-1488F49DB831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A7244B-FE69-4E67-89EA-40302DB537F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="214">
   <si>
     <t>bc_id</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>form_section_completion_instruction</t>
-  </si>
-  <si>
-    <t>QS_EQ5D02</t>
   </si>
   <si>
     <t>EQ-5D-5L Questionnaire</t>
@@ -791,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -829,7 +826,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,9 +961,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D10A2A-19A0-47CC-A5AB-F857D1ABF2BD}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K70" sqref="K70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -996,7 +992,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>32</v>
@@ -1026,7 +1022,7 @@
         <v>36</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1037,10 +1033,10 @@
         <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>31</v>
@@ -1055,7 +1051,7 @@
       <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>42</v>
       </c>
       <c r="K2" s="3" t="s">
@@ -1074,7 +1070,7 @@
         <v>37</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>39</v>
@@ -1092,7 +1088,7 @@
       <c r="I3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="K3" s="3" t="s">
@@ -1111,7 +1107,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>39</v>
@@ -1129,7 +1125,7 @@
       <c r="I4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="K4" s="3" t="s">
@@ -1148,7 +1144,7 @@
         <v>37</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>39</v>
@@ -1166,7 +1162,7 @@
       <c r="I5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="K5" s="3" t="s">
@@ -1185,7 +1181,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>39</v>
@@ -1203,7 +1199,7 @@
       <c r="I6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="K6" s="3" t="s">
@@ -1222,7 +1218,7 @@
         <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>39</v>
@@ -1240,7 +1236,7 @@
       <c r="I7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="12" t="s">
         <v>6</v>
       </c>
       <c r="K7" s="3" t="s">
@@ -1259,7 +1255,7 @@
         <v>37</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>39</v>
@@ -1277,7 +1273,7 @@
       <c r="I8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="12" t="s">
         <v>7</v>
       </c>
       <c r="K8" s="3" t="s">
@@ -1290,13 +1286,13 @@
     </row>
     <row r="9" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>40</v>
@@ -1314,7 +1310,7 @@
       <c r="I9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="12" t="s">
         <v>1</v>
       </c>
       <c r="K9" s="3" t="s">
@@ -1327,13 +1323,13 @@
     </row>
     <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>41</v>
@@ -1364,13 +1360,13 @@
     </row>
     <row r="11" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>41</v>
@@ -1386,10 +1382,10 @@
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>11</v>
@@ -1401,13 +1397,13 @@
     </row>
     <row r="12" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>41</v>
@@ -1438,13 +1434,13 @@
     </row>
     <row r="13" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>41</v>
@@ -1460,10 +1456,10 @@
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>11</v>
@@ -1475,13 +1471,13 @@
     </row>
     <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>41</v>
@@ -1497,10 +1493,10 @@
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>11</v>
@@ -1512,13 +1508,13 @@
     </row>
     <row r="15" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>41</v>
@@ -1549,19 +1545,19 @@
     </row>
     <row r="16" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E16" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="5">
         <v>1</v>
@@ -1570,10 +1566,10 @@
         <v>11</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>1</v>
@@ -1588,19 +1584,19 @@
     </row>
     <row r="17" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="5">
         <v>2</v>
@@ -1609,13 +1605,13 @@
         <v>11</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>11</v>
@@ -1627,19 +1623,19 @@
     </row>
     <row r="18" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="C18" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" s="5">
         <v>2</v>
@@ -1648,13 +1644,13 @@
         <v>11</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>11</v>
@@ -1666,19 +1662,19 @@
     </row>
     <row r="19" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F19" s="5">
         <v>2</v>
@@ -1687,13 +1683,13 @@
         <v>11</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>11</v>
@@ -1705,19 +1701,19 @@
     </row>
     <row r="20" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F20" s="5">
         <v>2</v>
@@ -1726,13 +1722,13 @@
         <v>11</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>11</v>
@@ -1744,19 +1740,19 @@
     </row>
     <row r="21" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="C21" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F21" s="5">
         <v>2</v>
@@ -1765,13 +1761,13 @@
         <v>11</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>11</v>
@@ -1783,19 +1779,19 @@
     </row>
     <row r="22" spans="1:13" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="C22" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="F22" s="5">
         <v>3</v>
@@ -1804,13 +1800,13 @@
         <v>11</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>11</v>
@@ -1822,19 +1818,19 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="E23" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F23" s="5">
         <v>1</v>
@@ -1842,9 +1838,9 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="J23" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J23" s="12" t="s">
         <v>1</v>
       </c>
       <c r="K23" s="3" t="s">
@@ -1857,19 +1853,19 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F24" s="5">
         <v>2</v>
@@ -1877,10 +1873,10 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>11</v>
@@ -1892,19 +1888,19 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F25" s="5">
         <v>2</v>
@@ -1912,10 +1908,10 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>11</v>
@@ -1927,19 +1923,19 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F26" s="5">
         <v>2</v>
@@ -1947,10 +1943,10 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>11</v>
@@ -1962,19 +1958,19 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F27" s="5">
         <v>2</v>
@@ -1982,10 +1978,10 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>11</v>
@@ -1997,19 +1993,19 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F28" s="5">
         <v>2</v>
@@ -2017,10 +2013,10 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>11</v>
@@ -2032,19 +2028,19 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F29" s="5">
         <v>2</v>
@@ -2052,10 +2048,10 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>11</v>
@@ -2067,19 +2063,19 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F30" s="5">
         <v>2</v>
@@ -2087,10 +2083,10 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>11</v>
@@ -2102,19 +2098,19 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F31" s="5">
         <v>2</v>
@@ -2122,10 +2118,10 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>11</v>
@@ -2137,19 +2133,19 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F32" s="5">
         <v>2</v>
@@ -2157,10 +2153,10 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>11</v>
@@ -2172,19 +2168,19 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F33" s="5">
         <v>1</v>
@@ -2192,10 +2188,10 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>11</v>
@@ -2207,19 +2203,19 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F34" s="5">
         <v>2</v>
@@ -2227,10 +2223,10 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J34" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>11</v>
@@ -2242,19 +2238,19 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F35" s="5">
         <v>3</v>
@@ -2262,10 +2258,10 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>11</v>
@@ -2277,19 +2273,19 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F36" s="5">
         <v>4</v>
@@ -2297,10 +2293,10 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>11</v>
@@ -2312,19 +2308,19 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F37" s="5">
         <v>5</v>
@@ -2332,10 +2328,10 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>11</v>
@@ -2347,19 +2343,19 @@
     </row>
     <row r="38" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F38" s="5">
         <v>6</v>
@@ -2367,10 +2363,10 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>11</v>
@@ -2382,19 +2378,19 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F39" s="5">
         <v>7</v>
@@ -2402,10 +2398,10 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="J39" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>11</v>
@@ -2417,19 +2413,19 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F40" s="5">
         <v>8</v>
@@ -2437,10 +2433,10 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>11</v>
@@ -2452,19 +2448,19 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F41" s="5">
         <v>9</v>
@@ -2472,10 +2468,10 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="J41" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>11</v>
@@ -2487,19 +2483,19 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F42" s="5">
         <v>10</v>
@@ -2507,10 +2503,10 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="J42" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>11</v>
@@ -2522,19 +2518,19 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F43" s="5">
         <v>11</v>
@@ -2542,10 +2538,10 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="J43" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>11</v>
@@ -2557,19 +2553,19 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F44" s="5">
         <v>12</v>
@@ -2577,10 +2573,10 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J44" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>11</v>
@@ -2592,19 +2588,19 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F45" s="5">
         <v>13</v>
@@ -2612,10 +2608,10 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="J45" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>11</v>
@@ -2627,19 +2623,19 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F46" s="5">
         <v>14</v>
@@ -2647,10 +2643,10 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="J46" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="K46" s="4" t="s">
         <v>11</v>
@@ -2662,19 +2658,19 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F47" s="5">
         <v>15</v>
@@ -2682,10 +2678,10 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="J47" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="K47" s="4" t="s">
         <v>11</v>
@@ -2697,19 +2693,19 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F48" s="5">
         <v>16</v>
@@ -2717,10 +2713,10 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="J48" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="K48" s="4" t="s">
         <v>11</v>
@@ -2732,19 +2728,19 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F49" s="5">
         <v>17</v>
@@ -2752,10 +2748,10 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="J49" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="K49" s="4" t="s">
         <v>11</v>
@@ -2767,19 +2763,19 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F50" s="5">
         <v>18</v>
@@ -2787,10 +2783,10 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="J50" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="K50" s="4" t="s">
         <v>11</v>
@@ -2802,19 +2798,19 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F51" s="5">
         <v>19</v>
@@ -2822,10 +2818,10 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="J51" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="K51" s="4" t="s">
         <v>11</v>
@@ -2837,19 +2833,19 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F52" s="5">
         <v>20</v>
@@ -2857,10 +2853,10 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="J52" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="K52" s="4" t="s">
         <v>11</v>
@@ -2872,19 +2868,19 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F53" s="5">
         <v>21</v>
@@ -2892,10 +2888,10 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="J53" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="K53" s="4" t="s">
         <v>11</v>
@@ -2907,19 +2903,19 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F54" s="5">
         <v>22</v>
@@ -2927,10 +2923,10 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="J54" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="K54" s="4" t="s">
         <v>11</v>
@@ -2942,19 +2938,19 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F55" s="5">
         <v>23</v>
@@ -2962,10 +2958,10 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="J55" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="K55" s="4" t="s">
         <v>11</v>
@@ -2977,19 +2973,19 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F56" s="5">
         <v>24</v>
@@ -2997,10 +2993,10 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="J56" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="K56" s="4" t="s">
         <v>11</v>
@@ -3012,19 +3008,19 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F57" s="5">
         <v>25</v>
@@ -3032,10 +3028,10 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="J57" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>199</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>11</v>
@@ -3047,19 +3043,19 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E58" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="F58" s="5">
         <v>26</v>
@@ -3067,10 +3063,10 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="J58" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="K58" s="4" t="s">
         <v>11</v>
@@ -3082,19 +3078,19 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F59" s="5">
         <v>27</v>
@@ -3102,10 +3098,10 @@
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="J59" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="J59" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="K59" s="4" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
update xslt + metadata
</commit_message>
<xml_diff>
--- a/metadata/cdisc_collection_forms.xlsx
+++ b/metadata/cdisc_collection_forms.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\lexjansen\cdisc360i-pocs\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A7244B-FE69-4E67-89EA-40302DB537F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B18855E-5655-4709-9256-847B2E854FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forms" sheetId="3" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forms!$A$1:$M$59</definedName>
+  </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="278">
   <si>
     <t>bc_id</t>
   </si>
@@ -101,9 +104,6 @@
     <t>EGPERF</t>
   </si>
   <si>
-    <t>EG</t>
-  </si>
-  <si>
     <t>EGHRMN_HORIZONTAL</t>
   </si>
   <si>
@@ -119,9 +119,6 @@
     <t>C117773</t>
   </si>
   <si>
-    <t>EG Performed</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
   </si>
   <si>
     <t>EQ-5D-5L Questionnaire - Lead Question</t>
-  </si>
-  <si>
-    <t>EQ-5D-5L Questionnaire - Question 1-4</t>
   </si>
   <si>
     <t>QS_EQ5D02_03</t>
@@ -325,105 +319,39 @@
     <t>VS1</t>
   </si>
   <si>
-    <t>ADAS-COG - Executive Function Maze Summary Score</t>
-  </si>
-  <si>
-    <t>ADASCOGSC_26</t>
-  </si>
-  <si>
     <t>ADAS-COG Summary Score</t>
   </si>
   <si>
     <t>ADASCOGSC1</t>
   </si>
   <si>
-    <t>ADAS-COG - Executive Function Maze: Time</t>
-  </si>
-  <si>
-    <t>ADASCOGSC_25</t>
-  </si>
-  <si>
-    <t>ADAS-COG - Executive Function Maze: Errors</t>
-  </si>
-  <si>
-    <t>ADASCOGSC_24</t>
-  </si>
-  <si>
-    <t>ADAS-COG - Number Cancellation Summary Score</t>
-  </si>
-  <si>
-    <t>ADASCOGSC_23</t>
-  </si>
-  <si>
-    <t>ADAS-COG - Number Cancellation: Remind</t>
-  </si>
-  <si>
-    <t>ADASCOGSC_22</t>
-  </si>
-  <si>
-    <t>ADAS-COG - Number Cancellation: Errors</t>
-  </si>
-  <si>
-    <t>ADASCOGSC_21</t>
-  </si>
-  <si>
-    <t>ADAS-COG - Number Cancellation: Correct</t>
-  </si>
-  <si>
-    <t>ADASCOGSC_20</t>
-  </si>
-  <si>
     <t>ADAS-COG - Concentration/Distractibility</t>
   </si>
   <si>
-    <t>ADASCOGSC_19</t>
-  </si>
-  <si>
     <t>ADAS-COG - Comprehension</t>
   </si>
   <si>
-    <t>ADASCOGSC_18</t>
-  </si>
-  <si>
     <t>ADAS-COG - Word Difficulty in Spontaneous Speech</t>
   </si>
   <si>
-    <t>ADASCOGSC_17</t>
-  </si>
-  <si>
     <t>ADAS-COG - Spoken Language Ability</t>
   </si>
   <si>
-    <t>ADASCOGSC_16</t>
-  </si>
-  <si>
     <t>ADAS-COG - Remembering Test Instructions</t>
   </si>
   <si>
     <t>ADASCOGSC_15</t>
   </si>
   <si>
-    <t>ADAS-COG - Word Recognition Summary Score</t>
-  </si>
-  <si>
     <t>ADASCOGSC_14</t>
   </si>
   <si>
-    <t>ADAS-COG - Word Recognition Trial 3 Subscore</t>
-  </si>
-  <si>
     <t>ADASCOGSC_13</t>
   </si>
   <si>
-    <t>ADAS-COG - Word Recognition Trial 2 Subscore</t>
-  </si>
-  <si>
     <t>ADASCOGSC_12</t>
   </si>
   <si>
-    <t>ADAS-COG - Word Recognition Trial 1 Subscore</t>
-  </si>
-  <si>
     <t>ADASCOGSC_11</t>
   </si>
   <si>
@@ -463,27 +391,15 @@
     <t>ADASCOGSC_05</t>
   </si>
   <si>
-    <t>ADAS-COG - Word Recall Average Score</t>
-  </si>
-  <si>
     <t>ADASCOGSC_04</t>
   </si>
   <si>
-    <t>ADAS-COG - Word Recall Trial 3 Subscore</t>
-  </si>
-  <si>
     <t>ADASCOGSC_03</t>
   </si>
   <si>
-    <t>ADAS-COG - Word Recall Trial 2 Subscore</t>
-  </si>
-  <si>
     <t>ADASCOGSC_02</t>
   </si>
   <si>
-    <t>ADAS-COG - Word Recall Trial 1 Subscore</t>
-  </si>
-  <si>
     <t>ADASCOGSC_01</t>
   </si>
   <si>
@@ -649,44 +565,334 @@
     <t>C100284</t>
   </si>
   <si>
+    <t>form_annotation</t>
+  </si>
+  <si>
+    <t>form_section_annotation</t>
+  </si>
+  <si>
+    <t>DOMAIN = FT; FTCAT = SIX MINUTE WALK</t>
+  </si>
+  <si>
+    <t>QRSAG_HORIZONTAL</t>
+  </si>
+  <si>
+    <t>C117779</t>
+  </si>
+  <si>
+    <t>QTCUNSAG_HORIZONTAL</t>
+  </si>
+  <si>
+    <t>C174285</t>
+  </si>
+  <si>
+    <t>QTAG_HORIZONTAL</t>
+  </si>
+  <si>
+    <t>C117783</t>
+  </si>
+  <si>
+    <t>ADASCOG_01</t>
+  </si>
+  <si>
+    <t>ADAS-COG - Word Recall</t>
+  </si>
+  <si>
+    <t>ADAS-COG - Word Recognition</t>
+  </si>
+  <si>
+    <t>ADAS-COG - Number Cancellation</t>
+  </si>
+  <si>
+    <t>ADAS-COG - Executive Function Maze</t>
+  </si>
+  <si>
     <t>ADASCOG</t>
   </si>
   <si>
-    <t>C100762</t>
-  </si>
-  <si>
-    <t>form_annotation</t>
-  </si>
-  <si>
-    <t>form_section_annotation</t>
-  </si>
-  <si>
-    <t>DOMAIN = FT; FTCAT = SIX MINUTE WALK</t>
-  </si>
-  <si>
-    <t>QRSAG_HORIZONTAL</t>
-  </si>
-  <si>
-    <t>C117779</t>
-  </si>
-  <si>
-    <t>QTCUNSAG_HORIZONTAL</t>
-  </si>
-  <si>
-    <t>C174285</t>
-  </si>
-  <si>
-    <t>QTAG_HORIZONTAL</t>
-  </si>
-  <si>
-    <t>C117783</t>
+    <t>ECG Performed</t>
+  </si>
+  <si>
+    <t>EQ-5D-5L Questionnaire - Question 1-5</t>
+  </si>
+  <si>
+    <t>DOMAIN = DM</t>
+  </si>
+  <si>
+    <t>DEMOG_LZZT</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS</t>
+  </si>
+  <si>
+    <t>BRTHDTC_DAT</t>
+  </si>
+  <si>
+    <t>C83217</t>
+  </si>
+  <si>
+    <t>SEX_MF</t>
+  </si>
+  <si>
+    <t>C28421</t>
+  </si>
+  <si>
+    <t>RACE</t>
+  </si>
+  <si>
+    <t>C17049</t>
+  </si>
+  <si>
+    <t>Demographics LZZT</t>
+  </si>
+  <si>
+    <t>IE_LZZT</t>
+  </si>
+  <si>
+    <t>Entry Procedures and Criteria for Enrollment</t>
+  </si>
+  <si>
+    <t>DOMAIN = IE</t>
+  </si>
+  <si>
+    <t>ENTRY_PROCEDURES</t>
+  </si>
+  <si>
+    <t>ENTRY PROCEDURES AND CRITERIA FOR ENROLLMENT</t>
+  </si>
+  <si>
+    <t>INCLEXCLYN</t>
+  </si>
+  <si>
+    <t>C83063</t>
+  </si>
+  <si>
+    <t>INCL01_SHORT_360</t>
+  </si>
+  <si>
+    <t>C25532</t>
+  </si>
+  <si>
+    <t>EXCL01_SHORT_360</t>
+  </si>
+  <si>
+    <t>C25370</t>
+  </si>
+  <si>
+    <t>EXPOSCOLL_XANOMELINEPLACEBO</t>
+  </si>
+  <si>
+    <t>Study Administration XANOMELINE or PLACEBO Daily Dose</t>
+  </si>
+  <si>
+    <t>DOMAIN = EC</t>
+  </si>
+  <si>
+    <t>EXPOSCOLL_XANPLAC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">STUDY DRUG </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>: DAILY PRESCRIBED DOSAGE</t>
+    </r>
+  </si>
+  <si>
+    <t>For this visit interval, record the number of patches (25-cm2 and 50-cm2 patches) that the patient is to wear per day.</t>
+  </si>
+  <si>
+    <t>EXPOSCOLL_XANOMELINEPLACEBO25</t>
+  </si>
+  <si>
+    <t>C117466</t>
+  </si>
+  <si>
+    <t>EXPOSCOLL_XANOMELINEPLACEBO50</t>
+  </si>
+  <si>
+    <t>MH_LZZT</t>
+  </si>
+  <si>
+    <t>Alzheimer's Disease</t>
+  </si>
+  <si>
+    <t>DOMAIN = MH</t>
+  </si>
+  <si>
+    <t>MH_AD_ONSET</t>
+  </si>
+  <si>
+    <t>PATIENT HISTORY : ALZHEIMER'S DISEASE ONSET DATE</t>
+  </si>
+  <si>
+    <t>Date of onset of the first definite symptoms of Alzheimer's Disease</t>
+  </si>
+  <si>
+    <t>MHALZHEIMERS_VERTICAL</t>
+  </si>
+  <si>
+    <t>C200145</t>
+  </si>
+  <si>
+    <t>PR_LZZT</t>
+  </si>
+  <si>
+    <t>Procedures</t>
+  </si>
+  <si>
+    <t>DOMAIN = PR</t>
+  </si>
+  <si>
+    <t>PR_CHESTXRAY</t>
+  </si>
+  <si>
+    <t>CHEST X-RAY</t>
+  </si>
+  <si>
+    <t>PR_SHORT_360</t>
+  </si>
+  <si>
+    <t>C87885</t>
+  </si>
+  <si>
+    <t>XRAYCHEST_SHORT</t>
+  </si>
+  <si>
+    <t>C38101</t>
+  </si>
+  <si>
+    <t>PR_MRI</t>
+  </si>
+  <si>
+    <t>PROCEDURE : MRI</t>
+  </si>
+  <si>
+    <t>MRIBRAIN_SHORT</t>
+  </si>
+  <si>
+    <t>C16809</t>
+  </si>
+  <si>
+    <t>PR_CTSCAN</t>
+  </si>
+  <si>
+    <t>PROCEDURE : CT SCAN</t>
+  </si>
+  <si>
+    <t>CTSCANCHEST_SHORT</t>
+  </si>
+  <si>
+    <t>C17204</t>
+  </si>
+  <si>
+    <t>SC_LZZT</t>
+  </si>
+  <si>
+    <t>Subject Characteristics Education LZZT</t>
+  </si>
+  <si>
+    <t>DOMAIN = SC</t>
+  </si>
+  <si>
+    <t>EDUCATION_LZZT</t>
+  </si>
+  <si>
+    <t>EDUCATION</t>
+  </si>
+  <si>
+    <t>EDUYRNUM</t>
+  </si>
+  <si>
+    <t>C122393</t>
+  </si>
+  <si>
+    <t>SU_LZZT</t>
+  </si>
+  <si>
+    <t>Substance Use Habits LZZT</t>
+  </si>
+  <si>
+    <t>SU_HABITS_SMOKING</t>
+  </si>
+  <si>
+    <t>HABITS : SMOKING</t>
+  </si>
+  <si>
+    <t>SU_360</t>
+  </si>
+  <si>
+    <t>NEW_2</t>
+  </si>
+  <si>
+    <t>SUCAT = TOBACCO</t>
+  </si>
+  <si>
+    <t>CIGARETTEHX_360</t>
+  </si>
+  <si>
+    <t>C181760</t>
+  </si>
+  <si>
+    <t>CIGARHX_360</t>
+  </si>
+  <si>
+    <t>PIPEHX_360</t>
+  </si>
+  <si>
+    <t>SU_HABITS_ALCOHOL</t>
+  </si>
+  <si>
+    <t>HABITS : ALCOHOL</t>
+  </si>
+  <si>
+    <t>SUCAT = ALCOHOL</t>
+  </si>
+  <si>
+    <t>BEERHX_360</t>
+  </si>
+  <si>
+    <t>C81229</t>
+  </si>
+  <si>
+    <t>DISTILLEDSPIRITSHX_360</t>
+  </si>
+  <si>
+    <t>WINEHX_360</t>
+  </si>
+  <si>
+    <t>SU_HABITS_CAFFEINE</t>
+  </si>
+  <si>
+    <t>HABITS : CAFFEINE</t>
+  </si>
+  <si>
+    <t>SUCAT = CAFFEINE</t>
+  </si>
+  <si>
+    <t>COFFEEHX_360</t>
+  </si>
+  <si>
+    <t>C201990</t>
+  </si>
+  <si>
+    <t>TEAHIX_360</t>
+  </si>
+  <si>
+    <t>COLAHX_360</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="9.5"/>
       <color rgb="FF000000"/>
@@ -702,6 +908,24 @@
       <sz val="9.5"/>
       <color rgb="FF000000"/>
       <name val="Albany AMT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Albany AMT"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -788,7 +1012,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -822,10 +1046,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,28 +1196,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D10A2A-19A0-47CC-A5AB-F857D1ABF2BD}">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="51" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" style="7" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="42.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26" style="2" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.28515625" style="2" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" style="10" customWidth="1"/>
-    <col min="13" max="13" width="33.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="31.140625" style="2" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -992,22 +1229,22 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>174</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>13</v>
@@ -1019,10 +1256,10 @@
         <v>12</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>206</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1030,16 +1267,16 @@
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>207</v>
+        <v>176</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F2" s="5">
         <v>1</v>
@@ -1051,8 +1288,8 @@
       <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="12" t="s">
-        <v>42</v>
+      <c r="J2" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>11</v>
@@ -1067,13 +1304,13 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
@@ -1088,7 +1325,7 @@
       <c r="I3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="K3" s="3" t="s">
@@ -1104,13 +1341,13 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>10</v>
@@ -1125,7 +1362,7 @@
       <c r="I4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="15" t="s">
         <v>3</v>
       </c>
       <c r="K4" s="3" t="s">
@@ -1141,13 +1378,13 @@
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>10</v>
@@ -1162,7 +1399,7 @@
       <c r="I5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="15" t="s">
         <v>4</v>
       </c>
       <c r="K5" s="3" t="s">
@@ -1178,13 +1415,13 @@
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>10</v>
@@ -1199,7 +1436,7 @@
       <c r="I6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="15" t="s">
         <v>5</v>
       </c>
       <c r="K6" s="3" t="s">
@@ -1215,13 +1452,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>10</v>
@@ -1236,7 +1473,7 @@
       <c r="I7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="15" t="s">
         <v>6</v>
       </c>
       <c r="K7" s="3" t="s">
@@ -1252,13 +1489,13 @@
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>10</v>
@@ -1273,7 +1510,7 @@
       <c r="I8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="15" t="s">
         <v>7</v>
       </c>
       <c r="K8" s="3" t="s">
@@ -1286,19 +1523,19 @@
     </row>
     <row r="9" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="E9" s="4" t="s">
-        <v>28</v>
+        <v>189</v>
       </c>
       <c r="F9" s="5">
         <v>1</v>
@@ -1310,7 +1547,7 @@
       <c r="I9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="15" t="s">
         <v>1</v>
       </c>
       <c r="K9" s="3" t="s">
@@ -1323,32 +1560,32 @@
     </row>
     <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F10" s="5">
         <v>2</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>11</v>
@@ -1360,32 +1597,32 @@
     </row>
     <row r="11" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F11" s="5">
         <v>2</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="12" t="s">
-        <v>208</v>
+      <c r="I11" s="11" t="s">
+        <v>177</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>209</v>
+        <v>178</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>11</v>
@@ -1397,32 +1634,32 @@
     </row>
     <row r="12" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F12" s="5">
         <v>2</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>11</v>
@@ -1434,32 +1671,32 @@
     </row>
     <row r="13" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F13" s="5">
         <v>2</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="12" t="s">
-        <v>212</v>
+      <c r="I13" s="11" t="s">
+        <v>181</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>213</v>
+        <v>182</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>11</v>
@@ -1471,32 +1708,32 @@
     </row>
     <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F14" s="5">
         <v>2</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="2" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>11</v>
@@ -1508,32 +1745,32 @@
     </row>
     <row r="15" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F15" s="5">
         <v>2</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>11</v>
@@ -1543,33 +1780,31 @@
       </c>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="F16" s="5">
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>1</v>
@@ -1584,34 +1819,34 @@
     </row>
     <row r="17" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E17" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F17" s="5">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="5">
-        <v>2</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="J17" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>11</v>
@@ -1623,34 +1858,34 @@
     </row>
     <row r="18" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F18" s="5">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="5">
-        <v>2</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="J18" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>11</v>
@@ -1662,34 +1897,34 @@
     </row>
     <row r="19" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E19" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F19" s="5">
+        <v>2</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="5">
-        <v>2</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="I19" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>11</v>
@@ -1701,34 +1936,34 @@
     </row>
     <row r="20" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E20" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F20" s="5">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="5">
-        <v>2</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="I20" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>11</v>
@@ -1740,34 +1975,34 @@
     </row>
     <row r="21" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E21" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F21" s="5">
+        <v>2</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="5">
-        <v>2</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="I21" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>11</v>
@@ -1779,19 +2014,19 @@
     </row>
     <row r="22" spans="1:13" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F22" s="5">
         <v>3</v>
@@ -1800,13 +2035,13 @@
         <v>11</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>11</v>
@@ -1818,19 +2053,19 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="F23" s="5">
         <v>1</v>
@@ -1838,9 +2073,9 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="J23" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J23" s="15" t="s">
         <v>1</v>
       </c>
       <c r="K23" s="3" t="s">
@@ -1853,19 +2088,19 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F24" s="5">
         <v>2</v>
@@ -1873,10 +2108,10 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>11</v>
@@ -1888,19 +2123,19 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F25" s="5">
         <v>2</v>
@@ -1908,10 +2143,10 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>11</v>
@@ -1923,19 +2158,19 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F26" s="5">
         <v>2</v>
@@ -1943,10 +2178,10 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>11</v>
@@ -1958,19 +2193,19 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F27" s="5">
         <v>2</v>
@@ -1978,10 +2213,10 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>11</v>
@@ -1993,19 +2228,19 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F28" s="5">
         <v>2</v>
@@ -2013,10 +2248,10 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>11</v>
@@ -2028,19 +2263,19 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F29" s="5">
         <v>2</v>
@@ -2048,10 +2283,10 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>11</v>
@@ -2063,19 +2298,19 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F30" s="5">
         <v>2</v>
@@ -2083,10 +2318,10 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>11</v>
@@ -2098,19 +2333,19 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F31" s="5">
         <v>2</v>
@@ -2118,10 +2353,10 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>11</v>
@@ -2133,19 +2368,19 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F32" s="5">
         <v>2</v>
@@ -2153,10 +2388,10 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>11</v>
@@ -2168,950 +2403,2071 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F33" s="5">
-        <v>1</v>
-      </c>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L33" s="3">
+        <v>120</v>
+      </c>
+      <c r="F33" s="4">
+        <v>1</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="4"/>
+      <c r="I33" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" s="4">
         <v>1</v>
       </c>
       <c r="M33" s="4"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F34" s="5">
-        <v>2</v>
-      </c>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L34" s="3">
-        <v>2</v>
+        <v>184</v>
+      </c>
+      <c r="F34" s="4">
+        <v>2</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="4"/>
+      <c r="I34" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L34" s="4">
+        <v>1</v>
       </c>
       <c r="M34" s="4"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F35" s="5">
-        <v>3</v>
-      </c>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>154</v>
+        <v>184</v>
+      </c>
+      <c r="F35" s="4">
+        <v>2</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="4"/>
+      <c r="I35" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L35" s="3">
-        <v>3</v>
+      <c r="L35" s="4">
+        <v>2</v>
       </c>
       <c r="M35" s="4"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F36" s="5">
-        <v>4</v>
-      </c>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>156</v>
+        <v>184</v>
+      </c>
+      <c r="F36" s="4">
+        <v>2</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="4"/>
+      <c r="I36" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>127</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L36" s="3">
-        <v>4</v>
+      <c r="L36" s="4">
+        <v>3</v>
       </c>
       <c r="M36" s="4"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F37" s="5">
-        <v>5</v>
-      </c>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>158</v>
+        <v>184</v>
+      </c>
+      <c r="F37" s="4">
+        <v>2</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="4"/>
+      <c r="I37" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>129</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L37" s="3">
-        <v>5</v>
+      <c r="L37" s="4">
+        <v>4</v>
       </c>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="F38" s="5">
-        <v>6</v>
-      </c>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>160</v>
+        <v>114</v>
+      </c>
+      <c r="F38" s="4">
+        <v>3</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="4"/>
+      <c r="I38" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>131</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L38" s="3">
-        <v>6</v>
+      <c r="L38" s="4">
+        <v>1</v>
       </c>
       <c r="M38" s="4"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="F39" s="5">
-        <v>7</v>
-      </c>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>162</v>
+        <v>112</v>
+      </c>
+      <c r="F39" s="4">
+        <v>4</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="4"/>
+      <c r="I39" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="J39" s="12" t="s">
+        <v>133</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L39" s="3">
-        <v>7</v>
+      <c r="L39" s="4">
+        <v>1</v>
       </c>
       <c r="M39" s="4"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="E40" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F40" s="4">
+        <v>5</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="4"/>
+      <c r="I40" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="J40" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="F40" s="5">
-        <v>8</v>
-      </c>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="K40" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L40" s="3">
-        <v>8</v>
+      <c r="L40" s="4">
+        <v>1</v>
       </c>
       <c r="M40" s="4"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F41" s="5">
-        <v>9</v>
-      </c>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>166</v>
+        <v>108</v>
+      </c>
+      <c r="F41" s="4">
+        <v>6</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="4"/>
+      <c r="I41" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="J41" s="12" t="s">
+        <v>137</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L41" s="3">
-        <v>9</v>
+      <c r="L41" s="4">
+        <v>1</v>
       </c>
       <c r="M41" s="4"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F42" s="5">
-        <v>10</v>
-      </c>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>168</v>
+        <v>106</v>
+      </c>
+      <c r="F42" s="4">
+        <v>7</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="4"/>
+      <c r="I42" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="J42" s="12" t="s">
+        <v>139</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L42" s="3">
-        <v>10</v>
+      <c r="L42" s="4">
+        <v>1</v>
       </c>
       <c r="M42" s="4"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F43" s="5">
-        <v>11</v>
-      </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>170</v>
+        <v>104</v>
+      </c>
+      <c r="F43" s="4">
+        <v>8</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="4"/>
+      <c r="I43" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>141</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L43" s="3">
-        <v>11</v>
+      <c r="L43" s="4">
+        <v>1</v>
       </c>
       <c r="M43" s="4"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F44" s="5">
-        <v>12</v>
-      </c>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>172</v>
+        <v>185</v>
+      </c>
+      <c r="F44" s="4">
+        <v>9</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="4"/>
+      <c r="I44" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>143</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L44" s="3">
-        <v>12</v>
+      <c r="L44" s="4">
+        <v>1</v>
       </c>
       <c r="M44" s="4"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F45" s="5">
-        <v>13</v>
-      </c>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>174</v>
+        <v>185</v>
+      </c>
+      <c r="F45" s="4">
+        <v>9</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="4"/>
+      <c r="I45" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J45" s="12" t="s">
+        <v>145</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L45" s="3">
-        <v>13</v>
+      <c r="L45" s="4">
+        <v>2</v>
       </c>
       <c r="M45" s="4"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F46" s="5">
-        <v>14</v>
-      </c>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>176</v>
+        <v>185</v>
+      </c>
+      <c r="F46" s="4">
+        <v>9</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="4"/>
+      <c r="I46" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="J46" s="12" t="s">
+        <v>147</v>
       </c>
       <c r="K46" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L46" s="3">
-        <v>14</v>
+      <c r="L46" s="4">
+        <v>3</v>
       </c>
       <c r="M46" s="4"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F47" s="5">
-        <v>15</v>
-      </c>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>178</v>
+        <v>185</v>
+      </c>
+      <c r="F47" s="4">
+        <v>9</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="4"/>
+      <c r="I47" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>149</v>
       </c>
       <c r="K47" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L47" s="3">
-        <v>15</v>
+      <c r="L47" s="4">
+        <v>4</v>
       </c>
       <c r="M47" s="4"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="4" t="s">
+      <c r="F48" s="4">
+        <v>10</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" s="4"/>
+      <c r="I48" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F48" s="5">
-        <v>16</v>
-      </c>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>180</v>
+      <c r="J48" s="12" t="s">
+        <v>151</v>
       </c>
       <c r="K48" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L48" s="3">
-        <v>16</v>
+      <c r="L48" s="4">
+        <v>1</v>
       </c>
       <c r="M48" s="4"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B49" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F49" s="5">
-        <v>17</v>
-      </c>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>182</v>
+      <c r="F49" s="4">
+        <v>11</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" s="4"/>
+      <c r="I49" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>153</v>
       </c>
       <c r="K49" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L49" s="3">
-        <v>17</v>
+      <c r="L49" s="4">
+        <v>1</v>
       </c>
       <c r="M49" s="4"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F50" s="5">
-        <v>18</v>
-      </c>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>184</v>
+        <v>96</v>
+      </c>
+      <c r="F50" s="4">
+        <v>12</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" s="4"/>
+      <c r="I50" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>155</v>
       </c>
       <c r="K50" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L50" s="3">
-        <v>18</v>
+      <c r="L50" s="4">
+        <v>1</v>
       </c>
       <c r="M50" s="4"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F51" s="5">
-        <v>19</v>
-      </c>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>186</v>
+        <v>95</v>
+      </c>
+      <c r="F51" s="4">
+        <v>13</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" s="4"/>
+      <c r="I51" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="K51" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L51" s="3">
-        <v>19</v>
+      <c r="L51" s="4">
+        <v>1</v>
       </c>
       <c r="M51" s="4"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F52" s="5">
-        <v>20</v>
-      </c>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>188</v>
+        <v>94</v>
+      </c>
+      <c r="F52" s="4">
+        <v>14</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" s="4"/>
+      <c r="I52" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>159</v>
       </c>
       <c r="K52" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L52" s="3">
-        <v>20</v>
+      <c r="L52" s="4">
+        <v>1</v>
       </c>
       <c r="M52" s="4"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F53" s="5">
-        <v>21</v>
-      </c>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="F53" s="4">
+        <v>15</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" s="4"/>
+      <c r="I53" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="J53" s="12" t="s">
+        <v>161</v>
       </c>
       <c r="K53" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L53" s="3">
-        <v>21</v>
+      <c r="L53" s="4">
+        <v>1</v>
       </c>
       <c r="M53" s="4"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F54" s="5">
-        <v>22</v>
-      </c>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
+      </c>
+      <c r="F54" s="4">
+        <v>15</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" s="4"/>
+      <c r="I54" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="J54" s="12" t="s">
+        <v>163</v>
       </c>
       <c r="K54" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L54" s="3">
-        <v>22</v>
+      <c r="L54" s="4">
+        <v>2</v>
       </c>
       <c r="M54" s="4"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F55" s="5">
-        <v>23</v>
-      </c>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>194</v>
+        <v>186</v>
+      </c>
+      <c r="F55" s="4">
+        <v>15</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="4"/>
+      <c r="I55" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="J55" s="12" t="s">
+        <v>165</v>
       </c>
       <c r="K55" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L55" s="3">
-        <v>23</v>
+      <c r="L55" s="4">
+        <v>3</v>
       </c>
       <c r="M55" s="4"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F56" s="5">
-        <v>24</v>
-      </c>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>196</v>
+        <v>186</v>
+      </c>
+      <c r="F56" s="4">
+        <v>15</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" s="4"/>
+      <c r="I56" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="J56" s="12" t="s">
+        <v>167</v>
       </c>
       <c r="K56" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L56" s="3">
-        <v>24</v>
+      <c r="L56" s="4">
+        <v>4</v>
       </c>
       <c r="M56" s="4"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F57" s="5">
-        <v>25</v>
-      </c>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>198</v>
+        <v>187</v>
+      </c>
+      <c r="F57" s="4">
+        <v>16</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" s="4"/>
+      <c r="I57" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="J57" s="12" t="s">
+        <v>169</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L57" s="3">
-        <v>25</v>
+      <c r="L57" s="4">
+        <v>1</v>
       </c>
       <c r="M57" s="4"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F58" s="5">
-        <v>26</v>
-      </c>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>200</v>
+        <v>187</v>
+      </c>
+      <c r="F58" s="4">
+        <v>16</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" s="4"/>
+      <c r="I58" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="J58" s="12" t="s">
+        <v>171</v>
       </c>
       <c r="K58" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L58" s="3">
-        <v>26</v>
+      <c r="L58" s="4">
+        <v>2</v>
       </c>
       <c r="M58" s="4"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F59" s="5">
-        <v>27</v>
-      </c>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="F59" s="4">
+        <v>16</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" s="4"/>
+      <c r="I59" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="J59" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L59" s="4">
+        <v>3</v>
+      </c>
+      <c r="M59" s="4"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="F60" s="13">
+        <v>1</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H60" s="13"/>
+      <c r="I60" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="J60" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="K60" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L60" s="13">
+        <v>1</v>
+      </c>
+      <c r="M60" s="13"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="F61" s="4">
+        <v>1</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" s="13"/>
+      <c r="I61" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="J61" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L61" s="4">
+        <v>2</v>
+      </c>
+      <c r="M61" s="4"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="F62" s="4">
+        <v>1</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H62" s="13"/>
+      <c r="I62" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="J62" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L62" s="4">
+        <v>3</v>
+      </c>
+      <c r="M62" s="4"/>
+    </row>
+    <row r="63" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="J59" s="2" t="s">
+      <c r="B63" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="K59" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L59" s="3">
-        <v>27</v>
-      </c>
-      <c r="M59" s="4"/>
+      <c r="C63" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="F63" s="13">
+        <v>1</v>
+      </c>
+      <c r="G63" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H63" s="13"/>
+      <c r="I63" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="J63" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="K63" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L63" s="13">
+        <v>1</v>
+      </c>
+      <c r="M63" s="13"/>
+    </row>
+    <row r="64" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="F64" s="13">
+        <v>1</v>
+      </c>
+      <c r="G64" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H64" s="13"/>
+      <c r="I64" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="J64" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="K64" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L64" s="13">
+        <v>2</v>
+      </c>
+      <c r="M64" s="13"/>
+    </row>
+    <row r="65" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="F65" s="13">
+        <v>1</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H65" s="13"/>
+      <c r="I65" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="J65" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="K65" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L65" s="13">
+        <v>3</v>
+      </c>
+      <c r="M65" s="13"/>
+    </row>
+    <row r="66" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="F66" s="13">
+        <v>1</v>
+      </c>
+      <c r="G66" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H66" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="I66" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="J66" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="K66" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L66" s="13">
+        <v>1</v>
+      </c>
+      <c r="M66" s="13"/>
+    </row>
+    <row r="67" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="F67" s="4">
+        <v>1</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H67" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="I67" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="J67" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="K67" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L67" s="4">
+        <v>2</v>
+      </c>
+      <c r="M67" s="4"/>
+    </row>
+    <row r="68" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A68" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="D68" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="F68" s="13">
+        <v>1</v>
+      </c>
+      <c r="G68" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H68" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="I68" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="J68" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="K68" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L68" s="13">
+        <v>1</v>
+      </c>
+      <c r="M68" s="13"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A69" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="F69" s="13">
+        <v>1</v>
+      </c>
+      <c r="G69" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H69" s="13"/>
+      <c r="I69" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="J69" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="K69" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L69" s="13">
+        <v>1</v>
+      </c>
+      <c r="M69" s="13"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A70" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="F70" s="13">
+        <v>1</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H70" s="13"/>
+      <c r="I70" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="J70" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="K70" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L70" s="13">
+        <v>2</v>
+      </c>
+      <c r="M70" s="13"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A71" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="F71" s="13">
+        <v>2</v>
+      </c>
+      <c r="G71" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H71" s="13"/>
+      <c r="I71" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="J71" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="K71" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L71" s="13">
+        <v>1</v>
+      </c>
+      <c r="M71" s="13"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A72" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="F72" s="13">
+        <v>2</v>
+      </c>
+      <c r="G72" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H72" s="13"/>
+      <c r="I72" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="J72" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="K72" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L72" s="13">
+        <v>2</v>
+      </c>
+      <c r="M72" s="13"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A73" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="D73" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="F73" s="13">
+        <v>3</v>
+      </c>
+      <c r="G73" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H73" s="13"/>
+      <c r="I73" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="J73" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="K73" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L73" s="13">
+        <v>1</v>
+      </c>
+      <c r="M73" s="13"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A74" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="E74" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="F74" s="13">
+        <v>3</v>
+      </c>
+      <c r="G74" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="J74" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="K74" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L74" s="13">
+        <v>2</v>
+      </c>
+      <c r="M74" s="13"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A75" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="F75" s="13">
+        <v>1</v>
+      </c>
+      <c r="G75" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H75" s="13"/>
+      <c r="I75" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="J75" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="K75" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L75" s="13">
+        <v>1</v>
+      </c>
+      <c r="M75" s="13"/>
+    </row>
+    <row r="76" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="E76" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="F76" s="13">
+        <v>1</v>
+      </c>
+      <c r="G76" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H76" s="13"/>
+      <c r="I76" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="J76" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="K76" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L76" s="13">
+        <v>1</v>
+      </c>
+      <c r="M76" s="13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A77" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D77" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="E77" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="F77" s="13">
+        <v>1</v>
+      </c>
+      <c r="G77" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H77" s="13"/>
+      <c r="I77" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="J77" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="K77" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L77" s="13">
+        <v>2</v>
+      </c>
+      <c r="M77" s="13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A78" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D78" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="E78" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="F78" s="13">
+        <v>1</v>
+      </c>
+      <c r="G78" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H78" s="13"/>
+      <c r="I78" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="J78" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="K78" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L78" s="13">
+        <v>3</v>
+      </c>
+      <c r="M78" s="13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A79" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C79" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="E79" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="F79" s="13">
+        <v>1</v>
+      </c>
+      <c r="G79" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H79" s="13"/>
+      <c r="I79" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="J79" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="K79" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L79" s="13">
+        <v>4</v>
+      </c>
+      <c r="M79" s="13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D80" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="E80" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="F80" s="13">
+        <v>2</v>
+      </c>
+      <c r="G80" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H80" s="13"/>
+      <c r="I80" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="J80" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="K80" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L80" s="13">
+        <v>1</v>
+      </c>
+      <c r="M80" s="13" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A81" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D81" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="E81" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="F81" s="13">
+        <v>2</v>
+      </c>
+      <c r="G81" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H81" s="13"/>
+      <c r="I81" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="J81" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="K81" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L81" s="13">
+        <v>2</v>
+      </c>
+      <c r="M81" s="13" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A82" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D82" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="E82" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="F82" s="13">
+        <v>2</v>
+      </c>
+      <c r="G82" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H82" s="13"/>
+      <c r="I82" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="J82" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="K82" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L82" s="13">
+        <v>3</v>
+      </c>
+      <c r="M82" s="13" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A83" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D83" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="F83" s="13">
+        <v>2</v>
+      </c>
+      <c r="G83" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H83" s="13"/>
+      <c r="I83" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="J83" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="K83" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L83" s="13">
+        <v>4</v>
+      </c>
+      <c r="M83" s="13" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C84" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D84" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="E84" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="F84" s="13">
+        <v>3</v>
+      </c>
+      <c r="G84" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H84" s="13"/>
+      <c r="I84" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="J84" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="K84" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L84" s="13">
+        <v>1</v>
+      </c>
+      <c r="M84" s="13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A85" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D85" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="E85" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="F85" s="13">
+        <v>3</v>
+      </c>
+      <c r="G85" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H85" s="13"/>
+      <c r="I85" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="J85" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="K85" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L85" s="13">
+        <v>2</v>
+      </c>
+      <c r="M85" s="13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A86" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D86" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="E86" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="F86" s="13">
+        <v>3</v>
+      </c>
+      <c r="G86" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H86" s="13"/>
+      <c r="I86" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="J86" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="K86" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L86" s="13">
+        <v>3</v>
+      </c>
+      <c r="M86" s="13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A87" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D87" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="F87" s="13">
+        <v>3</v>
+      </c>
+      <c r="G87" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H87" s="13"/>
+      <c r="I87" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="J87" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="K87" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L87" s="13">
+        <v>4</v>
+      </c>
+      <c r="M87" s="13" t="s">
+        <v>273</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M59" xr:uid="{11D10A2A-19A0-47CC-A5AB-F857D1ABF2BD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Forms metadata styling
</commit_message>
<xml_diff>
--- a/metadata/cdisc_collection_forms.xlsx
+++ b/metadata/cdisc_collection_forms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\lexjansen\cdisc360i-pocs\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09EA6BE-7B35-49C7-8A6D-6E423DD2DA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E50986-908B-424F-AAAB-D045F6463E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forms!$A$1:$M$59</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -892,7 +892,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="9.5"/>
       <color rgb="FF000000"/>
@@ -928,8 +928,14 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9.5"/>
+      <color rgb="FF112277"/>
+      <name val="Albany AMT"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -951,6 +957,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDF2F9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1012,7 +1024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1063,6 +1075,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1198,9 +1213,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D10A2A-19A0-47CC-A5AB-F857D1ABF2BD}">
   <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1231,19 +1246,19 @@
       <c r="C1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="18" t="s">
         <v>41</v>
       </c>
       <c r="I1" s="1" t="s">

</xml_diff>

<commit_message>
Add measurement units to ODM 1.3.2
</commit_message>
<xml_diff>
--- a/metadata/cdisc_collection_forms.xlsx
+++ b/metadata/cdisc_collection_forms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\lexjansen\cdisc360i-pocs\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C9D819-EF6E-4856-8329-13042A570E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FC9C4D-638A-4453-833E-74AC65E2F327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="915" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forms" sheetId="3" r:id="rId1"/>
@@ -854,6 +854,7 @@
       <sz val="9.5"/>
       <color rgb="FF000000"/>
       <name val="Albany AMT"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9.5"/>
@@ -865,6 +866,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Albany AMT"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -877,6 +879,7 @@
       <sz val="9.5"/>
       <color rgb="FF112277"/>
       <name val="Albany AMT"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -968,7 +971,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -984,23 +987,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1023,6 +1014,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1159,9 +1165,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D10A2A-19A0-47CC-A5AB-F857D1ABF2BD}">
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1171,14 +1177,14 @@
     <col min="3" max="3" width="33.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="46" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="17" customWidth="1"/>
     <col min="7" max="7" width="8.140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="22.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="33.5703125" style="2" customWidth="1"/>
     <col min="10" max="10" width="27.85546875" style="2" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" style="2" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="17" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -1192,22 +1198,22 @@
       <c r="C1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="13" t="s">
         <v>38</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1219,7 +1225,7 @@
       <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1239,7 +1245,7 @@
       <c r="E2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="16">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1250,13 +1256,13 @@
       <c r="J2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="11" t="s">
         <v>37</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1276,7 +1282,7 @@
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="16">
         <v>2</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -1287,13 +1293,13 @@
       <c r="J3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1313,7 +1319,7 @@
       <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="16">
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -1324,13 +1330,13 @@
       <c r="J4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="11" t="s">
         <v>3</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="16">
         <v>2</v>
       </c>
     </row>
@@ -1350,7 +1356,7 @@
       <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="16">
         <v>2</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -1361,13 +1367,13 @@
       <c r="J5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="16">
         <v>3</v>
       </c>
     </row>
@@ -1387,7 +1393,7 @@
       <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="16">
         <v>2</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -1398,13 +1404,13 @@
       <c r="J6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="16">
         <v>4</v>
       </c>
     </row>
@@ -1424,7 +1430,7 @@
       <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="16">
         <v>2</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -1435,13 +1441,13 @@
       <c r="J7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="16">
         <v>5</v>
       </c>
     </row>
@@ -1461,7 +1467,7 @@
       <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="16">
         <v>2</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -1472,13 +1478,13 @@
       <c r="J8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="16">
         <v>6</v>
       </c>
     </row>
@@ -1486,7 +1492,7 @@
       <c r="A9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1498,7 +1504,7 @@
       <c r="E9" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="16">
         <v>1</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -1509,13 +1515,13 @@
       <c r="J9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="11" t="s">
         <v>1</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1523,7 +1529,7 @@
       <c r="A10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1535,7 +1541,7 @@
       <c r="E10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="16">
         <v>2</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -1552,7 +1558,7 @@
       <c r="L10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1560,7 +1566,7 @@
       <c r="A11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1572,7 +1578,7 @@
       <c r="E11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="16">
         <v>2</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -1580,7 +1586,7 @@
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="7" t="s">
         <v>247</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -1589,7 +1595,7 @@
       <c r="L11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M11" s="3">
+      <c r="M11" s="16">
         <v>2</v>
       </c>
     </row>
@@ -1597,7 +1603,7 @@
       <c r="A12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1609,7 +1615,7 @@
       <c r="E12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="16">
         <v>2</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -1626,7 +1632,7 @@
       <c r="L12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M12" s="3">
+      <c r="M12" s="16">
         <v>3</v>
       </c>
     </row>
@@ -1634,7 +1640,7 @@
       <c r="A13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1646,7 +1652,7 @@
       <c r="E13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="16">
         <v>2</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -1654,7 +1660,7 @@
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="7" t="s">
         <v>249</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -1663,7 +1669,7 @@
       <c r="L13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13" s="16">
         <v>4</v>
       </c>
     </row>
@@ -1671,7 +1677,7 @@
       <c r="A14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1683,7 +1689,7 @@
       <c r="E14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="16">
         <v>2</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -1700,7 +1706,7 @@
       <c r="L14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M14" s="3">
+      <c r="M14" s="16">
         <v>5</v>
       </c>
     </row>
@@ -1708,7 +1714,7 @@
       <c r="A15" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1720,7 +1726,7 @@
       <c r="E15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="16">
         <v>2</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -1737,7 +1743,7 @@
       <c r="L15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15" s="16">
         <v>6</v>
       </c>
     </row>
@@ -1745,7 +1751,7 @@
       <c r="A16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -1757,7 +1763,7 @@
       <c r="E16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="16">
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -1774,7 +1780,7 @@
       <c r="L16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M16" s="3">
+      <c r="M16" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1782,7 +1788,7 @@
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1794,7 +1800,7 @@
       <c r="E17" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="16">
         <v>2</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -1813,7 +1819,7 @@
       <c r="L17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="3">
+      <c r="M17" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1821,7 +1827,7 @@
       <c r="A18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1833,7 +1839,7 @@
       <c r="E18" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="16">
         <v>2</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -1852,7 +1858,7 @@
       <c r="L18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M18" s="3">
+      <c r="M18" s="16">
         <v>2</v>
       </c>
     </row>
@@ -1860,7 +1866,7 @@
       <c r="A19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1872,7 +1878,7 @@
       <c r="E19" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="16">
         <v>2</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -1891,7 +1897,7 @@
       <c r="L19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M19" s="3">
+      <c r="M19" s="16">
         <v>3</v>
       </c>
     </row>
@@ -1899,7 +1905,7 @@
       <c r="A20" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1911,7 +1917,7 @@
       <c r="E20" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="16">
         <v>2</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -1930,7 +1936,7 @@
       <c r="L20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M20" s="3">
+      <c r="M20" s="16">
         <v>4</v>
       </c>
     </row>
@@ -1938,7 +1944,7 @@
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1950,7 +1956,7 @@
       <c r="E21" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="16">
         <v>2</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -1969,7 +1975,7 @@
       <c r="L21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M21" s="16">
         <v>5</v>
       </c>
     </row>
@@ -1977,7 +1983,7 @@
       <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1989,14 +1995,14 @@
       <c r="E22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="16">
         <v>3</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="5" t="s">
         <v>236</v>
       </c>
       <c r="J22" s="3" t="s">
@@ -2008,7 +2014,7 @@
       <c r="L22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M22" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2016,7 +2022,7 @@
       <c r="A23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -2028,7 +2034,7 @@
       <c r="E23" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="16">
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -2036,16 +2042,16 @@
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="8" t="s">
+      <c r="J23" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="K23" s="15" t="s">
+      <c r="K23" s="11" t="s">
         <v>1</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M23" s="3">
+      <c r="M23" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2053,7 +2059,7 @@
       <c r="A24" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -2065,7 +2071,7 @@
       <c r="E24" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="16">
         <v>2</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -2073,16 +2079,16 @@
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="8" t="s">
-        <v>245</v>
+      <c r="J24" s="6" t="s">
+        <v>240</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="3">
+      <c r="M24" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2090,7 +2096,7 @@
       <c r="A25" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -2102,7 +2108,7 @@
       <c r="E25" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="16">
         <v>2</v>
       </c>
       <c r="G25" s="3" t="s">
@@ -2110,16 +2116,16 @@
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="8" t="s">
-        <v>244</v>
+      <c r="J25" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M25" s="3">
+      <c r="M25" s="16">
         <v>2</v>
       </c>
     </row>
@@ -2127,7 +2133,7 @@
       <c r="A26" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -2139,7 +2145,7 @@
       <c r="E26" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="16">
         <v>2</v>
       </c>
       <c r="G26" s="3" t="s">
@@ -2147,16 +2153,16 @@
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="8" t="s">
-        <v>243</v>
+      <c r="J26" s="6" t="s">
+        <v>244</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M26" s="3">
+      <c r="M26" s="16">
         <v>3</v>
       </c>
     </row>
@@ -2164,7 +2170,7 @@
       <c r="A27" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2176,7 +2182,7 @@
       <c r="E27" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="16">
         <v>2</v>
       </c>
       <c r="G27" s="3" t="s">
@@ -2184,16 +2190,16 @@
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="8" t="s">
-        <v>242</v>
+      <c r="J27" s="6" t="s">
+        <v>245</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M27" s="3">
+      <c r="M27" s="16">
         <v>4</v>
       </c>
     </row>
@@ -2201,7 +2207,7 @@
       <c r="A28" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -2213,7 +2219,7 @@
       <c r="E28" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="16">
         <v>2</v>
       </c>
       <c r="G28" s="3" t="s">
@@ -2221,16 +2227,16 @@
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="8" t="s">
-        <v>241</v>
+      <c r="J28" s="6" t="s">
+        <v>243</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M28" s="3">
+      <c r="M28" s="16">
         <v>5</v>
       </c>
     </row>
@@ -2238,7 +2244,7 @@
       <c r="A29" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -2250,7 +2256,7 @@
       <c r="E29" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="16">
         <v>2</v>
       </c>
       <c r="G29" s="3" t="s">
@@ -2258,16 +2264,16 @@
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="8" t="s">
-        <v>240</v>
+      <c r="J29" s="6" t="s">
+        <v>241</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="L29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M29" s="3">
+      <c r="M29" s="16">
         <v>6</v>
       </c>
     </row>
@@ -2275,7 +2281,7 @@
       <c r="A30" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -2287,7 +2293,7 @@
       <c r="E30" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="16">
         <v>2</v>
       </c>
       <c r="G30" s="3" t="s">
@@ -2295,16 +2301,16 @@
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-      <c r="J30" s="8" t="s">
-        <v>239</v>
+      <c r="J30" s="6" t="s">
+        <v>238</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M30" s="3">
+      <c r="M30" s="16">
         <v>7</v>
       </c>
     </row>
@@ -2312,7 +2318,7 @@
       <c r="A31" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -2324,7 +2330,7 @@
       <c r="E31" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="16">
         <v>2</v>
       </c>
       <c r="G31" s="3" t="s">
@@ -2332,16 +2338,16 @@
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="8" t="s">
-        <v>237</v>
+      <c r="J31" s="6" t="s">
+        <v>242</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M31" s="3">
+      <c r="M31" s="16">
         <v>8</v>
       </c>
     </row>
@@ -2349,7 +2355,7 @@
       <c r="A32" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -2361,7 +2367,7 @@
       <c r="E32" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="16">
         <v>2</v>
       </c>
       <c r="G32" s="3" t="s">
@@ -2369,16 +2375,16 @@
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
-      <c r="J32" s="8" t="s">
-        <v>238</v>
+      <c r="J32" s="6" t="s">
+        <v>237</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M32" s="3">
+      <c r="M32" s="16">
         <v>9</v>
       </c>
     </row>
@@ -2398,7 +2404,7 @@
       <c r="E33" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="16">
         <v>1</v>
       </c>
       <c r="G33" s="4" t="s">
@@ -2406,16 +2412,16 @@
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
-      <c r="J33" s="12" t="s">
+      <c r="J33" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="K33" s="12" t="s">
+      <c r="K33" s="8" t="s">
         <v>1</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M33" s="4">
+      <c r="M33" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2435,7 +2441,7 @@
       <c r="E34" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="16">
         <v>2</v>
       </c>
       <c r="G34" s="4" t="s">
@@ -2443,16 +2449,16 @@
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
-      <c r="J34" s="12" t="s">
+      <c r="J34" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="K34" s="12" t="s">
+      <c r="K34" s="8" t="s">
         <v>110</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M34" s="4">
+      <c r="M34" s="16">
         <v>4</v>
       </c>
     </row>
@@ -2472,7 +2478,7 @@
       <c r="E35" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="16">
         <v>3</v>
       </c>
       <c r="G35" s="4" t="s">
@@ -2480,16 +2486,16 @@
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
-      <c r="J35" s="12" t="s">
+      <c r="J35" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="K35" s="12" t="s">
+      <c r="K35" s="8" t="s">
         <v>112</v>
       </c>
       <c r="L35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M35" s="4">
+      <c r="M35" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2509,7 +2515,7 @@
       <c r="E36" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="16">
         <v>4</v>
       </c>
       <c r="G36" s="4" t="s">
@@ -2517,16 +2523,16 @@
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
-      <c r="J36" s="12" t="s">
+      <c r="J36" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="K36" s="12" t="s">
+      <c r="K36" s="8" t="s">
         <v>114</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M36" s="4">
+      <c r="M36" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2546,7 +2552,7 @@
       <c r="E37" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="16">
         <v>5</v>
       </c>
       <c r="G37" s="4" t="s">
@@ -2554,16 +2560,16 @@
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="12" t="s">
+      <c r="J37" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="K37" s="12" t="s">
+      <c r="K37" s="8" t="s">
         <v>116</v>
       </c>
       <c r="L37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M37" s="4">
+      <c r="M37" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2583,7 +2589,7 @@
       <c r="E38" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="16">
         <v>6</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -2591,16 +2597,16 @@
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="12" t="s">
+      <c r="J38" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="K38" s="12" t="s">
+      <c r="K38" s="8" t="s">
         <v>118</v>
       </c>
       <c r="L38" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M38" s="4">
+      <c r="M38" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2620,7 +2626,7 @@
       <c r="E39" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="16">
         <v>7</v>
       </c>
       <c r="G39" s="4" t="s">
@@ -2628,16 +2634,16 @@
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
-      <c r="J39" s="12" t="s">
+      <c r="J39" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="K39" s="12" t="s">
+      <c r="K39" s="8" t="s">
         <v>120</v>
       </c>
       <c r="L39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M39" s="4">
+      <c r="M39" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2657,7 +2663,7 @@
       <c r="E40" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F40" s="4">
+      <c r="F40" s="16">
         <v>8</v>
       </c>
       <c r="G40" s="4" t="s">
@@ -2665,16 +2671,16 @@
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="12" t="s">
+      <c r="J40" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="K40" s="12" t="s">
+      <c r="K40" s="8" t="s">
         <v>122</v>
       </c>
       <c r="L40" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M40" s="4">
+      <c r="M40" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2694,7 +2700,7 @@
       <c r="E41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F41" s="16">
         <v>9</v>
       </c>
       <c r="G41" s="4" t="s">
@@ -2702,16 +2708,16 @@
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="12" t="s">
+      <c r="J41" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="K41" s="12" t="s">
+      <c r="K41" s="8" t="s">
         <v>124</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M41" s="4">
+      <c r="M41" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2731,7 +2737,7 @@
       <c r="E42" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="4">
+      <c r="F42" s="16">
         <v>10</v>
       </c>
       <c r="G42" s="4" t="s">
@@ -2739,16 +2745,16 @@
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
-      <c r="J42" s="12" t="s">
+      <c r="J42" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="K42" s="12" t="s">
+      <c r="K42" s="8" t="s">
         <v>126</v>
       </c>
       <c r="L42" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M42" s="4">
+      <c r="M42" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2768,7 +2774,7 @@
       <c r="E43" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F43" s="16">
         <v>11</v>
       </c>
       <c r="G43" s="4" t="s">
@@ -2776,16 +2782,16 @@
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="12" t="s">
+      <c r="J43" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="K43" s="12" t="s">
+      <c r="K43" s="8" t="s">
         <v>128</v>
       </c>
       <c r="L43" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M43" s="4">
+      <c r="M43" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2805,7 +2811,7 @@
       <c r="E44" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F44" s="16">
         <v>12</v>
       </c>
       <c r="G44" s="4" t="s">
@@ -2813,16 +2819,16 @@
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="12" t="s">
+      <c r="J44" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="K44" s="12" t="s">
+      <c r="K44" s="8" t="s">
         <v>130</v>
       </c>
       <c r="L44" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M44" s="4">
+      <c r="M44" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2842,7 +2848,7 @@
       <c r="E45" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F45" s="4">
+      <c r="F45" s="16">
         <v>13</v>
       </c>
       <c r="G45" s="4" t="s">
@@ -2850,16 +2856,16 @@
       </c>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="12" t="s">
+      <c r="J45" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="K45" s="12" t="s">
+      <c r="K45" s="8" t="s">
         <v>132</v>
       </c>
       <c r="L45" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M45" s="4">
+      <c r="M45" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2879,7 +2885,7 @@
       <c r="E46" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F46" s="4">
+      <c r="F46" s="16">
         <v>14</v>
       </c>
       <c r="G46" s="4" t="s">
@@ -2887,16 +2893,16 @@
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="12" t="s">
+      <c r="J46" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="K46" s="12" t="s">
+      <c r="K46" s="8" t="s">
         <v>134</v>
       </c>
       <c r="L46" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M46" s="4">
+      <c r="M46" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2916,7 +2922,7 @@
       <c r="E47" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F47" s="16">
         <v>15</v>
       </c>
       <c r="G47" s="4" t="s">
@@ -2924,16 +2930,16 @@
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
-      <c r="J47" s="12" t="s">
+      <c r="J47" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="K47" s="12" t="s">
+      <c r="K47" s="8" t="s">
         <v>136</v>
       </c>
       <c r="L47" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M47" s="4">
+      <c r="M47" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2953,7 +2959,7 @@
       <c r="E48" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F48" s="4">
+      <c r="F48" s="16">
         <v>16</v>
       </c>
       <c r="G48" s="4" t="s">
@@ -2961,16 +2967,16 @@
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
-      <c r="J48" s="12" t="s">
+      <c r="J48" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="K48" s="12" t="s">
+      <c r="K48" s="8" t="s">
         <v>138</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M48" s="4">
+      <c r="M48" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2990,7 +2996,7 @@
       <c r="E49" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F49" s="4">
+      <c r="F49" s="16">
         <v>16</v>
       </c>
       <c r="G49" s="4" t="s">
@@ -2998,1193 +3004,1193 @@
       </c>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
-      <c r="J49" s="12" t="s">
+      <c r="J49" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="K49" s="12" t="s">
+      <c r="K49" s="8" t="s">
         <v>140</v>
       </c>
       <c r="L49" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M49" s="4">
+      <c r="M49" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E50" s="13" t="s">
+      <c r="E50" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="F50" s="13">
-        <v>1</v>
-      </c>
-      <c r="G50" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="12" t="s">
+      <c r="F50" s="18">
+        <v>1</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="K50" s="15" t="s">
+      <c r="K50" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="L50" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M50" s="13">
+      <c r="L50" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M50" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D51" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E51" s="13" t="s">
+      <c r="E51" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F51" s="16">
         <v>1</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H51" s="4"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="12" t="s">
+      <c r="I51" s="9"/>
+      <c r="J51" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="K51" s="15" t="s">
+      <c r="K51" s="11" t="s">
         <v>160</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M51" s="4">
+      <c r="M51" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D52" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E52" s="13" t="s">
+      <c r="E52" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="F52" s="4">
+      <c r="F52" s="16">
         <v>1</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H52" s="4"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="12" t="s">
+      <c r="I52" s="9"/>
+      <c r="J52" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="K52" s="15" t="s">
+      <c r="K52" s="11" t="s">
         <v>162</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M52" s="4">
+      <c r="M52" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D53" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E53" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F53" s="13">
-        <v>1</v>
-      </c>
-      <c r="G53" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="11" t="s">
+      <c r="F53" s="18">
+        <v>1</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="K53" s="15" t="s">
+      <c r="K53" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="L53" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M53" s="13">
+      <c r="L53" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M53" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="D54" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E54" s="13" t="s">
+      <c r="E54" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F54" s="13">
-        <v>1</v>
-      </c>
-      <c r="G54" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="11" t="s">
+      <c r="F54" s="18">
+        <v>1</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="K54" s="15" t="s">
+      <c r="K54" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="L54" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M54" s="13">
+      <c r="L54" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M54" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C55" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D55" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E55" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F55" s="13">
-        <v>1</v>
-      </c>
-      <c r="G55" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="8" t="s">
+      <c r="F55" s="18">
+        <v>1</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="K55" s="15" t="s">
+      <c r="K55" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="L55" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M55" s="13">
+      <c r="L55" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M55" s="18">
         <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C56" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="D56" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="E56" s="13" t="s">
+      <c r="E56" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="F56" s="13">
-        <v>1</v>
-      </c>
-      <c r="G56" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="18" t="s">
+      <c r="F56" s="18">
+        <v>1</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="K56" s="15" t="s">
+      <c r="K56" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="L56" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M56" s="13">
+      <c r="L56" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M56" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C57" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D57" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="E57" s="13" t="s">
+      <c r="E57" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="F57" s="13">
-        <v>2</v>
-      </c>
-      <c r="G57" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13" t="s">
+      <c r="F57" s="18">
+        <v>2</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="J57" s="14" t="s">
+      <c r="J57" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="K57" s="16" t="s">
+      <c r="K57" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="L57" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M57" s="13">
+      <c r="L57" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M57" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="9" t="s">
         <v>175</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D58" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="E58" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="F58" s="4">
+      <c r="F58" s="16">
         <v>2</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H58" s="4"/>
-      <c r="I58" s="13" t="s">
+      <c r="I58" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="J58" s="14" t="s">
+      <c r="J58" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="K58" s="13" t="s">
+      <c r="K58" s="9" t="s">
         <v>180</v>
       </c>
       <c r="L58" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M58" s="4">
+      <c r="M58" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="D59" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="E59" s="13" t="s">
+      <c r="E59" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="F59" s="4">
+      <c r="F59" s="16">
         <v>1</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H59" s="4"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="14" t="s">
+      <c r="I59" s="9"/>
+      <c r="J59" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="K59" s="13" t="s">
+      <c r="K59" s="9" t="s">
         <v>262</v>
       </c>
       <c r="L59" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M59" s="4">
+      <c r="M59" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="D60" s="13" t="s">
+      <c r="D60" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="E60" s="13" t="s">
+      <c r="E60" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F60" s="13">
-        <v>2</v>
-      </c>
-      <c r="G60" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H60" s="13"/>
-      <c r="I60" s="13" t="s">
+      <c r="F60" s="18">
+        <v>2</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="J60" s="13" t="s">
+      <c r="J60" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="K60" s="13" t="s">
+      <c r="K60" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="L60" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M60" s="13">
+      <c r="L60" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M60" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="D61" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="E61" s="13" t="s">
+      <c r="E61" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="F61" s="13">
-        <v>1</v>
-      </c>
-      <c r="G61" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H61" s="13"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="11" t="s">
+      <c r="F61" s="18">
+        <v>1</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="K61" s="11" t="s">
+      <c r="K61" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="L61" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M61" s="13">
+      <c r="L61" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M61" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C62" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="D62" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="E62" s="13" t="s">
+      <c r="E62" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="F62" s="13">
-        <v>1</v>
-      </c>
-      <c r="G62" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="11" t="s">
+      <c r="F62" s="18">
+        <v>1</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="K62" s="11" t="s">
+      <c r="K62" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="L62" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M62" s="13">
+      <c r="L62" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M62" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C63" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D63" s="13" t="s">
+      <c r="D63" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="E63" s="13" t="s">
+      <c r="E63" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="F63" s="13">
-        <v>2</v>
-      </c>
-      <c r="G63" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="11" t="s">
+      <c r="F63" s="18">
+        <v>2</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="K63" s="11" t="s">
+      <c r="K63" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="L63" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M63" s="13">
+      <c r="L63" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M63" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B64" s="13" t="s">
+      <c r="B64" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="C64" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D64" s="13" t="s">
+      <c r="D64" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="E64" s="13" t="s">
+      <c r="E64" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="F64" s="13">
-        <v>2</v>
-      </c>
-      <c r="G64" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="11" t="s">
+      <c r="F64" s="18">
+        <v>2</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="K64" s="11" t="s">
+      <c r="K64" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="L64" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M64" s="13">
+      <c r="L64" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M64" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A65" s="13" t="s">
+      <c r="A65" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B65" s="13" t="s">
+      <c r="B65" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C65" s="13" t="s">
+      <c r="C65" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D65" s="13" t="s">
+      <c r="D65" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="E65" s="13" t="s">
+      <c r="E65" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="F65" s="13">
+      <c r="F65" s="18">
         <v>3</v>
       </c>
-      <c r="G65" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="11" t="s">
+      <c r="G65" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="K65" s="11" t="s">
+      <c r="K65" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="L65" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M65" s="13">
+      <c r="L65" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M65" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B66" s="13" t="s">
+      <c r="B66" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="C66" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D66" s="13" t="s">
+      <c r="D66" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="E66" s="13" t="s">
+      <c r="E66" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="F66" s="13">
+      <c r="F66" s="18">
         <v>3</v>
       </c>
-      <c r="G66" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H66" s="13"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="13" t="s">
+      <c r="G66" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="K66" s="13" t="s">
+      <c r="K66" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="L66" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M66" s="13">
+      <c r="L66" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M66" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A67" s="13" t="s">
+      <c r="A67" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="C67" s="13" t="s">
+      <c r="C67" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D67" s="13" t="s">
+      <c r="D67" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="E67" s="13" t="s">
+      <c r="E67" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="F67" s="13">
-        <v>1</v>
-      </c>
-      <c r="G67" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H67" s="13"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="11" t="s">
+      <c r="F67" s="18">
+        <v>1</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="K67" s="11" t="s">
+      <c r="K67" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="L67" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M67" s="13">
+      <c r="L67" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M67" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A68" s="13" t="s">
+      <c r="A68" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B68" s="13" t="s">
+      <c r="B68" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="C68" s="13" t="s">
+      <c r="C68" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D68" s="13" t="s">
+      <c r="D68" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="E68" s="13" t="s">
+      <c r="E68" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="F68" s="13">
-        <v>1</v>
-      </c>
-      <c r="G68" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="11" t="s">
+      <c r="F68" s="18">
+        <v>1</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="K68" s="11" t="s">
+      <c r="K68" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="L68" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M68" s="13">
+      <c r="L68" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M68" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A69" s="13" t="s">
+      <c r="A69" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B69" s="13" t="s">
+      <c r="B69" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C69" s="13" t="s">
+      <c r="C69" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D69" s="13" t="s">
+      <c r="D69" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="E69" s="13" t="s">
+      <c r="E69" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="F69" s="13">
-        <v>1</v>
-      </c>
-      <c r="G69" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H69" s="13" t="s">
+      <c r="F69" s="18">
+        <v>1</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H69" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="I69" s="13"/>
-      <c r="J69" s="11" t="s">
+      <c r="I69" s="9"/>
+      <c r="J69" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="K69" s="11" t="s">
+      <c r="K69" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="L69" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M69" s="13">
+      <c r="L69" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M69" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A70" s="13" t="s">
+      <c r="A70" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C70" s="13" t="s">
+      <c r="C70" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D70" s="13" t="s">
+      <c r="D70" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="E70" s="13" t="s">
+      <c r="E70" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="F70" s="13">
-        <v>1</v>
-      </c>
-      <c r="G70" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H70" s="13" t="s">
+      <c r="F70" s="18">
+        <v>1</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H70" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="I70" s="13"/>
-      <c r="J70" s="11" t="s">
+      <c r="I70" s="9"/>
+      <c r="J70" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="K70" s="11" t="s">
+      <c r="K70" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="L70" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M70" s="13">
+      <c r="L70" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M70" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A71" s="13" t="s">
+      <c r="A71" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="C71" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D71" s="13" t="s">
+      <c r="D71" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="E71" s="13" t="s">
+      <c r="E71" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="F71" s="13">
-        <v>1</v>
-      </c>
-      <c r="G71" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H71" s="13" t="s">
+      <c r="F71" s="18">
+        <v>1</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H71" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="I71" s="13"/>
-      <c r="J71" s="11" t="s">
+      <c r="I71" s="9"/>
+      <c r="J71" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="K71" s="11" t="s">
+      <c r="K71" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="L71" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M71" s="13">
+      <c r="L71" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M71" s="18">
         <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A72" s="13" t="s">
+      <c r="A72" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="C72" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D72" s="13" t="s">
+      <c r="D72" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="E72" s="13" t="s">
+      <c r="E72" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="F72" s="13">
-        <v>1</v>
-      </c>
-      <c r="G72" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H72" s="13" t="s">
+      <c r="F72" s="18">
+        <v>1</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H72" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="I72" s="13"/>
-      <c r="J72" s="11" t="s">
+      <c r="I72" s="9"/>
+      <c r="J72" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="K72" s="11" t="s">
+      <c r="K72" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="L72" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M72" s="13">
+      <c r="L72" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M72" s="18">
         <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A73" s="13" t="s">
+      <c r="A73" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B73" s="13" t="s">
+      <c r="B73" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="C73" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D73" s="13" t="s">
+      <c r="D73" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="E73" s="13" t="s">
+      <c r="E73" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="F73" s="13">
-        <v>2</v>
-      </c>
-      <c r="G73" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H73" s="13" t="s">
+      <c r="F73" s="18">
+        <v>2</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H73" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="I73" s="13"/>
-      <c r="J73" s="11" t="s">
+      <c r="I73" s="9"/>
+      <c r="J73" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="K73" s="11" t="s">
+      <c r="K73" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="L73" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M73" s="13">
+      <c r="L73" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M73" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A74" s="13" t="s">
+      <c r="A74" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B74" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C74" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D74" s="13" t="s">
+      <c r="D74" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="E74" s="13" t="s">
+      <c r="E74" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="F74" s="13">
-        <v>2</v>
-      </c>
-      <c r="G74" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H74" s="13" t="s">
+      <c r="F74" s="18">
+        <v>2</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H74" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="I74" s="13"/>
-      <c r="J74" s="11" t="s">
+      <c r="I74" s="9"/>
+      <c r="J74" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="K74" s="11" t="s">
+      <c r="K74" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="L74" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M74" s="13">
+      <c r="L74" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M74" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A75" s="13" t="s">
+      <c r="A75" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B75" s="13" t="s">
+      <c r="B75" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C75" s="13" t="s">
+      <c r="C75" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D75" s="13" t="s">
+      <c r="D75" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="E75" s="13" t="s">
+      <c r="E75" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="F75" s="13">
-        <v>2</v>
-      </c>
-      <c r="G75" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H75" s="13" t="s">
+      <c r="F75" s="18">
+        <v>2</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H75" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="I75" s="13"/>
-      <c r="J75" s="11" t="s">
+      <c r="I75" s="9"/>
+      <c r="J75" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="K75" s="11" t="s">
+      <c r="K75" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="L75" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M75" s="13">
+      <c r="L75" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M75" s="18">
         <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B76" s="13" t="s">
+      <c r="B76" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C76" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D76" s="13" t="s">
+      <c r="D76" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="E76" s="13" t="s">
+      <c r="E76" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="F76" s="13">
-        <v>2</v>
-      </c>
-      <c r="G76" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H76" s="13" t="s">
+      <c r="F76" s="18">
+        <v>2</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H76" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="I76" s="13"/>
-      <c r="J76" s="11" t="s">
+      <c r="I76" s="9"/>
+      <c r="J76" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="K76" s="11" t="s">
+      <c r="K76" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="L76" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M76" s="13">
+      <c r="L76" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M76" s="18">
         <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A77" s="13" t="s">
+      <c r="A77" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B77" s="13" t="s">
+      <c r="B77" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C77" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D77" s="13" t="s">
+      <c r="D77" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E77" s="13" t="s">
+      <c r="E77" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="F77" s="13">
+      <c r="F77" s="18">
         <v>3</v>
       </c>
-      <c r="G77" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H77" s="13" t="s">
+      <c r="G77" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H77" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="I77" s="13"/>
-      <c r="J77" s="11" t="s">
+      <c r="I77" s="9"/>
+      <c r="J77" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="K77" s="11" t="s">
+      <c r="K77" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="L77" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M77" s="13">
+      <c r="L77" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M77" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A78" s="13" t="s">
+      <c r="A78" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B78" s="13" t="s">
+      <c r="B78" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C78" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D78" s="13" t="s">
+      <c r="D78" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E78" s="13" t="s">
+      <c r="E78" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="F78" s="13">
+      <c r="F78" s="18">
         <v>3</v>
       </c>
-      <c r="G78" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H78" s="13" t="s">
+      <c r="G78" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H78" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="I78" s="13"/>
-      <c r="J78" s="11" t="s">
+      <c r="I78" s="9"/>
+      <c r="J78" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="K78" s="11" t="s">
+      <c r="K78" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="L78" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M78" s="13">
+      <c r="L78" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M78" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A79" s="13" t="s">
+      <c r="A79" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B79" s="13" t="s">
+      <c r="B79" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C79" s="13" t="s">
+      <c r="C79" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D79" s="13" t="s">
+      <c r="D79" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E79" s="13" t="s">
+      <c r="E79" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="F79" s="13">
+      <c r="F79" s="18">
         <v>3</v>
       </c>
-      <c r="G79" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H79" s="13" t="s">
+      <c r="G79" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H79" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="I79" s="13"/>
-      <c r="J79" s="11" t="s">
+      <c r="I79" s="9"/>
+      <c r="J79" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="K79" s="11" t="s">
+      <c r="K79" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="L79" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M79" s="13">
+      <c r="L79" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M79" s="18">
         <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A80" s="13" t="s">
+      <c r="A80" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B80" s="13" t="s">
+      <c r="B80" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C80" s="13" t="s">
+      <c r="C80" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D80" s="13" t="s">
+      <c r="D80" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E80" s="13" t="s">
+      <c r="E80" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="F80" s="13">
+      <c r="F80" s="18">
         <v>3</v>
       </c>
-      <c r="G80" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H80" s="13" t="s">
+      <c r="G80" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H80" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="I80" s="13"/>
-      <c r="J80" s="11" t="s">
+      <c r="I80" s="9"/>
+      <c r="J80" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="K80" s="11" t="s">
+      <c r="K80" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="L80" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M80" s="13">
+      <c r="L80" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M80" s="18">
         <v>4</v>
       </c>
     </row>

</xml_diff>